<commit_message>
Small fix and a restart
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>EBIT</t>
   </si>
@@ -29,6 +29,27 @@
   </si>
   <si>
     <t>CY</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
   </si>
 </sst>
 </file>
@@ -410,25 +431,123 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3468716000</v>
+      </c>
+      <c r="C2">
+        <v>3720356000</v>
+      </c>
+      <c r="D2">
+        <v>1100000000</v>
+      </c>
+      <c r="E2">
+        <v>8333000</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>4469282000</v>
+      </c>
+      <c r="C3">
+        <v>555913000</v>
+      </c>
+      <c r="D3">
+        <v>2050000000</v>
+      </c>
+      <c r="E3">
+        <v>-3298000</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>5373593000</v>
+      </c>
+      <c r="C4">
+        <v>-1696013000</v>
+      </c>
+      <c r="D4">
+        <v>2750000000</v>
+      </c>
+      <c r="E4">
+        <v>114959000</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>6587000000</v>
+      </c>
+      <c r="C5">
+        <v>2634000000</v>
+      </c>
+      <c r="D5">
+        <v>3050000000</v>
+      </c>
+      <c r="E5">
+        <v>73000000</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>8514000000</v>
+      </c>
+      <c r="C6">
+        <v>1719000000</v>
+      </c>
+      <c r="D6">
+        <v>3950000000</v>
+      </c>
+      <c r="E6">
+        <v>96000000</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>9254000000</v>
+      </c>
+      <c r="C7">
+        <v>868000000</v>
+      </c>
+      <c r="D7">
+        <v>7068000000</v>
+      </c>
+      <c r="E7">
+        <v>51000000</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>10291000000</v>
+      </c>
+      <c r="C8">
+        <v>2833000000</v>
+      </c>
+      <c r="D8">
+        <v>4400000000</v>
+      </c>
+      <c r="E8">
+        <v>-156000000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished the calcs, wc ratios missing
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>EBIT</t>
   </si>
   <si>
+    <t>op income</t>
+  </si>
+  <si>
     <t>working capital</t>
   </si>
   <si>
@@ -28,7 +31,58 @@
     <t>interest expense</t>
   </si>
   <si>
+    <t>sales growth</t>
+  </si>
+  <si>
+    <t>gp margin</t>
+  </si>
+  <si>
+    <t>EBITDA margin</t>
+  </si>
+  <si>
+    <t>EBIT margin</t>
+  </si>
+  <si>
+    <t>wc turnover</t>
+  </si>
+  <si>
+    <t>receivables turnover</t>
+  </si>
+  <si>
+    <t>inventory turnover</t>
+  </si>
+  <si>
+    <t>payables turnover</t>
+  </si>
+  <si>
+    <t>gross profit</t>
+  </si>
+  <si>
+    <t>EBITDA</t>
+  </si>
+  <si>
+    <t>net debt</t>
+  </si>
+  <si>
+    <t>leverage</t>
+  </si>
+  <si>
+    <t>wc ratio</t>
+  </si>
+  <si>
+    <t>solvency ratio</t>
+  </si>
+  <si>
+    <t>interest cover</t>
+  </si>
+  <si>
     <t>CY</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
   </si>
   <si>
     <t>2017</t>
@@ -407,15 +461,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -429,124 +483,527 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B2">
+        <v>1836033000</v>
+      </c>
+      <c r="C2">
+        <v>1591803000</v>
+      </c>
+      <c r="D2">
+        <v>2608336000</v>
+      </c>
+      <c r="E2">
+        <v>625000000</v>
+      </c>
+      <c r="F2">
+        <v>35425000</v>
+      </c>
+      <c r="H2">
+        <v>0.844788803528967</v>
+      </c>
+      <c r="I2">
+        <v>0.4536546783022706</v>
+      </c>
+      <c r="J2">
+        <v>0.3828649334763282</v>
+      </c>
+      <c r="O2">
+        <v>4051194000</v>
+      </c>
+      <c r="P2">
+        <v>2175506000</v>
+      </c>
+      <c r="Q2">
+        <v>-2972063000</v>
+      </c>
+      <c r="R2">
+        <v>-1.366147921449079</v>
+      </c>
+      <c r="S2">
+        <v>2.178346515742091</v>
+      </c>
+      <c r="T2">
+        <v>-0.6498099131815174</v>
+      </c>
+      <c r="U2">
+        <v>51.82873676781934</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>2546615000</v>
+      </c>
+      <c r="C3">
+        <v>2280259000</v>
+      </c>
+      <c r="D3">
+        <v>3028139000</v>
+      </c>
+      <c r="E3">
+        <v>1075000000</v>
+      </c>
+      <c r="F3">
+        <v>23102000</v>
+      </c>
+      <c r="G3">
+        <v>1.220814632684609</v>
+      </c>
+      <c r="H3">
+        <v>0.8599508406454599</v>
+      </c>
+      <c r="I3">
+        <v>0.491619167023946</v>
+      </c>
+      <c r="J3">
+        <v>0.4349894011885017</v>
+      </c>
+      <c r="O3">
+        <v>5034522000</v>
+      </c>
+      <c r="P3">
+        <v>2878150000</v>
+      </c>
+      <c r="Q3">
+        <v>-2874296000</v>
+      </c>
+      <c r="R3">
+        <v>-0.9986609453989542</v>
+      </c>
+      <c r="S3">
+        <v>2.077002882664357</v>
+      </c>
+      <c r="T3">
+        <v>-0.9086725932193483</v>
+      </c>
+      <c r="U3">
+        <v>110.2335295645399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
         <v>3468716000</v>
       </c>
-      <c r="C2">
+      <c r="C4">
+        <v>3025029000</v>
+      </c>
+      <c r="D4">
         <v>3720356000</v>
       </c>
-      <c r="D2">
+      <c r="E4">
         <v>1100000000</v>
       </c>
-      <c r="E2">
+      <c r="F4">
         <v>8333000</v>
       </c>
+      <c r="G4">
+        <v>1.247176070087096</v>
+      </c>
+      <c r="H4">
+        <v>0.8616051074401784</v>
+      </c>
+      <c r="I4">
+        <v>0.5197165515876522</v>
+      </c>
+      <c r="J4">
+        <v>0.475068633110571</v>
+      </c>
+      <c r="O4">
+        <v>6291014000</v>
+      </c>
+      <c r="P4">
+        <v>3794713000</v>
+      </c>
+      <c r="Q4">
+        <v>-1520516000</v>
+      </c>
+      <c r="R4">
+        <v>-0.400693280361387</v>
+      </c>
+      <c r="S4">
+        <v>2.054685003956108</v>
+      </c>
+      <c r="T4">
+        <v>-2.203874211123066</v>
+      </c>
+      <c r="U4">
+        <v>416.2625705028201</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
+    <row r="5" spans="1:21">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
         <v>4469282000</v>
       </c>
-      <c r="C3">
+      <c r="C5">
+        <v>4266180000</v>
+      </c>
+      <c r="D5">
         <v>555913000</v>
       </c>
-      <c r="D3">
+      <c r="E5">
         <v>2050000000</v>
       </c>
-      <c r="E3">
+      <c r="F5">
         <v>-3298000</v>
       </c>
+      <c r="G5">
+        <v>1.236732427081814</v>
+      </c>
+      <c r="H5">
+        <v>0.8676635723910765</v>
+      </c>
+      <c r="I5">
+        <v>0.5333078331713549</v>
+      </c>
+      <c r="J5">
+        <v>0.4949366600782635</v>
+      </c>
+      <c r="O5">
+        <v>7835009000</v>
+      </c>
+      <c r="P5">
+        <v>4815774000</v>
+      </c>
+      <c r="Q5">
+        <v>-2575259000</v>
+      </c>
+      <c r="R5">
+        <v>-0.5347549532017075</v>
+      </c>
+      <c r="S5">
+        <v>1.129248248016915</v>
+      </c>
+      <c r="T5">
+        <v>-1.791148773773822</v>
+      </c>
+      <c r="U5">
+        <v>-1355.149181322013</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
+    <row r="6" spans="1:21">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
         <v>5373593000</v>
       </c>
-      <c r="C4">
+      <c r="C6">
+        <v>5120310000</v>
+      </c>
+      <c r="D6">
         <v>-1696013000</v>
       </c>
-      <c r="D4">
+      <c r="E6">
         <v>2750000000</v>
       </c>
-      <c r="E4">
+      <c r="F6">
         <v>114959000</v>
       </c>
+      <c r="G6">
+        <v>1.23713035470179</v>
+      </c>
+      <c r="H6">
+        <v>0.8502662672024565</v>
+      </c>
+      <c r="I6">
+        <v>0.5469608408047875</v>
+      </c>
+      <c r="J6">
+        <v>0.4810178263096935</v>
+      </c>
+      <c r="O6">
+        <v>9498577000</v>
+      </c>
+      <c r="P6">
+        <v>6110262000</v>
+      </c>
+      <c r="Q6">
+        <v>-1488046000</v>
+      </c>
+      <c r="R6">
+        <v>-0.243532274066153</v>
+      </c>
+      <c r="S6">
+        <v>0.7929403201440421</v>
+      </c>
+      <c r="T6">
+        <v>-3.936020123033831</v>
+      </c>
+      <c r="U6">
+        <v>46.74356074774485</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
+    <row r="7" spans="1:21">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
         <v>6587000000</v>
       </c>
-      <c r="C5">
+      <c r="C7">
+        <v>7671000000</v>
+      </c>
+      <c r="D7">
         <v>2634000000</v>
       </c>
-      <c r="D5">
+      <c r="E7">
         <v>3050000000</v>
       </c>
-      <c r="E5">
+      <c r="F7">
         <v>73000000</v>
       </c>
+      <c r="G7">
+        <v>1.151880573938729</v>
+      </c>
+      <c r="H7">
+        <v>0.8661796705004663</v>
+      </c>
+      <c r="I7">
+        <v>0.5774790177183712</v>
+      </c>
+      <c r="J7">
+        <v>0.5118899595896799</v>
+      </c>
+      <c r="O7">
+        <v>11146000000</v>
+      </c>
+      <c r="P7">
+        <v>7431000000</v>
+      </c>
+      <c r="Q7">
+        <v>-821000000</v>
+      </c>
+      <c r="R7">
+        <v>-0.1104831112905396</v>
+      </c>
+      <c r="S7">
+        <v>1.477866473149492</v>
+      </c>
+      <c r="T7">
+        <v>-10.37149817295981</v>
+      </c>
+      <c r="U7">
+        <v>90.23287671232876</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
+    <row r="8" spans="1:21">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
         <v>8514000000</v>
       </c>
-      <c r="C6">
+      <c r="C8">
+        <v>7631000000</v>
+      </c>
+      <c r="D8">
         <v>1719000000</v>
       </c>
-      <c r="D6">
+      <c r="E8">
         <v>3950000000</v>
       </c>
-      <c r="E6">
+      <c r="F8">
         <v>96000000</v>
       </c>
+      <c r="G8">
+        <v>1.226686353745726</v>
+      </c>
+      <c r="H8">
+        <v>0.8818498574596135</v>
+      </c>
+      <c r="I8">
+        <v>0.5939182768451061</v>
+      </c>
+      <c r="J8">
+        <v>0.5393728222996516</v>
+      </c>
+      <c r="O8">
+        <v>13920000000</v>
+      </c>
+      <c r="P8">
+        <v>9375000000</v>
+      </c>
+      <c r="Q8">
+        <v>-1379000000</v>
+      </c>
+      <c r="R8">
+        <v>-0.1470933333333333</v>
+      </c>
+      <c r="S8">
+        <v>1.24798038084247</v>
+      </c>
+      <c r="T8">
+        <v>-6.158085569253082</v>
+      </c>
+      <c r="U8">
+        <v>88.6875</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
+    <row r="9" spans="1:21">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
         <v>9254000000</v>
       </c>
-      <c r="C7">
+      <c r="C9">
+        <v>8002000000</v>
+      </c>
+      <c r="D9">
         <v>868000000</v>
       </c>
-      <c r="D7">
+      <c r="E9">
         <v>7068000000</v>
       </c>
-      <c r="E7">
+      <c r="F9">
         <v>51000000</v>
       </c>
+      <c r="G9">
+        <v>1.115362686094393</v>
+      </c>
+      <c r="H9">
+        <v>0.8770305577643985</v>
+      </c>
+      <c r="I9">
+        <v>0.5789503578325571</v>
+      </c>
+      <c r="J9">
+        <v>0.5256162671816427</v>
+      </c>
+      <c r="O9">
+        <v>15441000000</v>
+      </c>
+      <c r="P9">
+        <v>10193000000</v>
+      </c>
+      <c r="Q9">
+        <v>-901000000</v>
+      </c>
+      <c r="R9">
+        <v>-0.08839399587952516</v>
+      </c>
+      <c r="S9">
+        <v>1.106791338582677</v>
+      </c>
+      <c r="T9">
+        <v>-9.923418423973363</v>
+      </c>
+      <c r="U9">
+        <v>181.4509803921569</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
+    <row r="10" spans="1:21">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
         <v>10291000000</v>
       </c>
-      <c r="C8">
+      <c r="C10">
+        <v>8920000000</v>
+      </c>
+      <c r="D10">
         <v>2833000000</v>
       </c>
-      <c r="D8">
+      <c r="E10">
         <v>4400000000</v>
       </c>
-      <c r="E8">
+      <c r="F10">
         <v>-156000000</v>
+      </c>
+      <c r="G10">
+        <v>1.102408269907986</v>
+      </c>
+      <c r="H10">
+        <v>0.878716059559998</v>
+      </c>
+      <c r="I10">
+        <v>0.578855170281828</v>
+      </c>
+      <c r="J10">
+        <v>0.5302179401308671</v>
+      </c>
+      <c r="O10">
+        <v>17055000000</v>
+      </c>
+      <c r="P10">
+        <v>11235000000</v>
+      </c>
+      <c r="Q10">
+        <v>2615000000</v>
+      </c>
+      <c r="R10">
+        <v>0.2327547841566533</v>
+      </c>
+      <c r="S10">
+        <v>1.343352320930796</v>
+      </c>
+      <c r="T10">
+        <v>3.77208413001912</v>
+      </c>
+      <c r="U10">
+        <v>-65.96794871794872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>